<commit_message>
organzing code to review errors in data
</commit_message>
<xml_diff>
--- a/model-configurations.xlsx
+++ b/model-configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiyenggar/code/regioncitations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795D975D-30E1-3948-938C-C1D4929675DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF62F781-E141-3240-9800-1CC9279261F0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41200" yWindow="2240" windowWidth="25440" windowHeight="14380" activeTab="1" xr2:uid="{768EC7B8-1B86-FB40-9549-9FB99E4420DB}"/>
+    <workbookView xWindow="-41200" yWindow="2240" windowWidth="25440" windowHeight="14380" xr2:uid="{768EC7B8-1B86-FB40-9549-9FB99E4420DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" r:id="rId1"/>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2AACB43-532C-9A4E-AE59-984A73CC0A00}">
   <dimension ref="B2:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D53580-1244-B64F-8AD4-BBB8E90644A2}">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>